<commit_message>
Added more data + visualizations + standardized
</commit_message>
<xml_diff>
--- a/math_proj.xlsx
+++ b/math_proj.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charumathibadrinath/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charumathibadrinath/Logistic_Regression_Math_22b/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C4E6DB-419A-6843-BDB3-2E00C718D63A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823EF5B9-F74B-C641-AAD4-74AD2D269AE5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{11B802F1-FAA6-0B4B-A3A1-7B10C2516FEB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{11B802F1-FAA6-0B4B-A3A1-7B10C2516FEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
-    <t>Country </t>
-  </si>
-  <si>
     <t>Real GDP growth</t>
   </si>
   <si>
@@ -313,6 +310,9 @@
   </si>
   <si>
     <t>Class</t>
+  </si>
+  <si>
+    <t>Country</t>
   </si>
 </sst>
 </file>
@@ -678,32 +678,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8A22F13-6111-9245-ADF6-F392717258C4}">
   <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="173" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>2.2000000000000002</v>
@@ -721,7 +719,7 @@
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>1.4</v>
@@ -739,7 +737,7 @@
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>1.4</v>
@@ -757,7 +755,7 @@
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>1.7</v>
@@ -775,7 +773,7 @@
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>2.8</v>
@@ -793,7 +791,7 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>3.7</v>
@@ -811,7 +809,7 @@
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>2.9</v>
@@ -829,7 +827,7 @@
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>2.2999999999999998</v>
@@ -847,7 +845,7 @@
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>2.9</v>
@@ -865,7 +863,7 @@
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>5</v>
@@ -883,7 +881,7 @@
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>1.3</v>
@@ -901,7 +899,7 @@
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>1.5</v>
@@ -919,7 +917,7 @@
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <v>0.6</v>
@@ -937,7 +935,7 @@
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15">
         <v>1.9</v>
@@ -955,7 +953,7 @@
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>4.5999999999999996</v>
@@ -973,7 +971,7 @@
     </row>
     <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17">
         <v>2.6</v>
@@ -991,7 +989,7 @@
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>5.9</v>
@@ -1009,7 +1007,7 @@
     </row>
     <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>0.3</v>
@@ -1027,7 +1025,7 @@
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -1045,7 +1043,7 @@
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>4.3</v>
@@ -1063,7 +1061,7 @@
     </row>
     <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22">
         <v>2.2999999999999998</v>
@@ -1081,7 +1079,7 @@
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23">
         <v>5.5</v>
@@ -1099,7 +1097,7 @@
     </row>
     <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24">
         <v>4.0999999999999996</v>
@@ -1117,7 +1115,7 @@
     </row>
     <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25">
         <v>1.7</v>
@@ -1135,7 +1133,7 @@
     </row>
     <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26">
         <v>3.2</v>
@@ -1153,7 +1151,7 @@
     </row>
     <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27">
         <v>0.9</v>
@@ -1171,7 +1169,7 @@
     </row>
     <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B28">
         <v>4.5</v>
@@ -1189,7 +1187,7 @@
     </row>
     <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29">
         <v>2.5</v>
@@ -1207,7 +1205,7 @@
     </row>
     <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30">
         <v>4.0999999999999996</v>
@@ -1225,7 +1223,7 @@
     </row>
     <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -1243,7 +1241,7 @@
     </row>
     <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B32">
         <v>4.2</v>
@@ -1261,7 +1259,7 @@
     </row>
     <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B33">
         <v>2.2999999999999998</v>
@@ -1279,7 +1277,7 @@
     </row>
     <row r="34" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B34">
         <v>3.2</v>
@@ -1297,7 +1295,7 @@
     </row>
     <row r="35" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35">
         <v>2</v>
@@ -1315,7 +1313,7 @@
     </row>
     <row r="36" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B36">
         <v>1.4</v>
@@ -1333,7 +1331,7 @@
     </row>
     <row r="37" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B37">
         <v>1.1000000000000001</v>
@@ -1351,7 +1349,7 @@
     </row>
     <row r="38" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B38">
         <v>3.2</v>
@@ -1369,7 +1367,7 @@
     </row>
     <row r="39" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B39">
         <v>1.4</v>
@@ -1387,7 +1385,7 @@
     </row>
     <row r="40" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B40">
         <v>0.8</v>
@@ -1405,7 +1403,7 @@
     </row>
     <row r="41" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41">
         <v>-0.6</v>
@@ -1423,7 +1421,7 @@
     </row>
     <row r="42" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B42">
         <v>6.9</v>
@@ -1441,7 +1439,7 @@
     </row>
     <row r="43" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B43">
         <v>3</v>
@@ -1459,7 +1457,7 @@
     </row>
     <row r="44" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B44">
         <v>5.7</v>
@@ -1477,7 +1475,7 @@
     </row>
     <row r="45" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B45">
         <v>1.8</v>
@@ -1495,7 +1493,7 @@
     </row>
     <row r="46" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B46">
         <v>5.7</v>
@@ -1513,7 +1511,7 @@
     </row>
     <row r="47" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B47">
         <v>3.9</v>
@@ -1531,7 +1529,7 @@
     </row>
     <row r="48" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B48">
         <v>3</v>
@@ -1549,7 +1547,7 @@
     </row>
     <row r="49" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B49">
         <v>3</v>
@@ -1567,7 +1565,7 @@
     </row>
     <row r="50" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B50">
         <v>1.9</v>
@@ -1585,7 +1583,7 @@
     </row>
     <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B51">
         <v>4.4000000000000004</v>
@@ -1603,7 +1601,7 @@
     </row>
     <row r="52" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B52">
         <v>6.2</v>
@@ -1621,7 +1619,7 @@
     </row>
     <row r="53" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B53">
         <v>7.5</v>
@@ -1639,7 +1637,7 @@
     </row>
     <row r="54" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B54">
         <v>5.6</v>
@@ -1657,7 +1655,7 @@
     </row>
     <row r="55" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B55">
         <f>D44</f>
@@ -1676,7 +1674,7 @@
     </row>
     <row r="56" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B56">
         <v>3.8</v>
@@ -1694,7 +1692,7 @@
     </row>
     <row r="57" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B57">
         <v>2.2000000000000002</v>
@@ -1712,7 +1710,7 @@
     </row>
     <row r="58" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B58">
         <v>9</v>
@@ -1730,7 +1728,7 @@
     </row>
     <row r="59" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B59">
         <v>3.9</v>
@@ -1748,7 +1746,7 @@
     </row>
     <row r="60" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B60">
         <v>6.1</v>
@@ -1766,7 +1764,7 @@
     </row>
     <row r="61" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B61">
         <v>6.5</v>
@@ -1784,7 +1782,7 @@
     </row>
     <row r="62" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B62">
         <v>5.6</v>
@@ -1802,7 +1800,7 @@
     </row>
     <row r="63" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B63">
         <v>4.5</v>
@@ -1820,7 +1818,7 @@
     </row>
     <row r="64" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B64">
         <v>5.4</v>
@@ -1838,7 +1836,7 @@
     </row>
     <row r="65" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B65">
         <v>1.1000000000000001</v>
@@ -1856,7 +1854,7 @@
     </row>
     <row r="66" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B66">
         <v>-2.5</v>
@@ -1874,7 +1872,7 @@
     </row>
     <row r="67" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B67">
         <v>13.2</v>
@@ -1892,7 +1890,7 @@
     </row>
     <row r="68" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B68">
         <v>4.4000000000000004</v>
@@ -1910,7 +1908,7 @@
     </row>
     <row r="69" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B69">
         <v>4.5</v>
@@ -1928,7 +1926,7 @@
     </row>
     <row r="70" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B70">
         <v>4.8</v>
@@ -1946,7 +1944,7 @@
     </row>
     <row r="71" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B71">
         <v>5.6</v>
@@ -1964,7 +1962,7 @@
     </row>
     <row r="72" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B72">
         <v>3</v>
@@ -1982,7 +1980,7 @@
     </row>
     <row r="73" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B73">
         <v>2.5</v>
@@ -2000,7 +1998,7 @@
     </row>
     <row r="74" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B74">
         <v>2.2999999999999998</v>
@@ -2018,7 +2016,7 @@
     </row>
     <row r="75" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B75">
         <v>-1.6</v>
@@ -2036,7 +2034,7 @@
     </row>
     <row r="76" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B76">
         <v>5.9</v>
@@ -2054,7 +2052,7 @@
     </row>
     <row r="77" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B77">
         <v>2.2000000000000002</v>
@@ -2072,7 +2070,7 @@
     </row>
     <row r="78" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B78">
         <v>9.4</v>
@@ -2090,7 +2088,7 @@
     </row>
     <row r="79" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B79">
         <v>4.4000000000000004</v>
@@ -2108,7 +2106,7 @@
     </row>
     <row r="80" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B80">
         <v>1.9</v>
@@ -2126,7 +2124,7 @@
     </row>
     <row r="81" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B81">
         <v>5.5</v>
@@ -2144,7 +2142,7 @@
     </row>
     <row r="82" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B82">
         <v>0.2</v>
@@ -2162,7 +2160,7 @@
     </row>
     <row r="83" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B83">
         <v>0.9</v>
@@ -2180,7 +2178,7 @@
     </row>
     <row r="84" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B84">
         <v>-2.5</v>
@@ -2198,7 +2196,7 @@
     </row>
     <row r="85" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B85">
         <v>5.5</v>
@@ -2216,7 +2214,7 @@
     </row>
     <row r="86" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -2234,7 +2232,7 @@
     </row>
     <row r="87" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B87">
         <v>8</v>
@@ -2252,7 +2250,7 @@
     </row>
     <row r="88" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B88">
         <v>1.4</v>
@@ -2270,7 +2268,7 @@
     </row>
     <row r="89" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B89">
         <v>-7.4</v>

</xml_diff>